<commit_message>
Finalized rev 2.2 m52 board
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev2.2 documents/BOM-speeduino compatible PCB for m52 rev2.2.xlsx
+++ b/m52 PnP/Rev2.2 documents/BOM-speeduino compatible PCB for m52 rev2.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev2.2 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314DE61F-AA7F-44A2-B7B5-8B44D81AFAE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C1240-75ED-4943-A37D-6FB18D3D3328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="0" windowWidth="26985" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="780" windowWidth="26985" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -1237,22 +1237,22 @@
     <t>DIY-EFI.uk</t>
   </si>
   <si>
-    <t>6-POS connector</t>
-  </si>
-  <si>
-    <t>6 CKT RCPT HOUSING</t>
-  </si>
-  <si>
-    <t>39-01-2060</t>
-  </si>
-  <si>
-    <t>WM3702-ND</t>
-  </si>
-  <si>
-    <t>538-39-01-2060</t>
-  </si>
-  <si>
     <t>Wideband connector</t>
+  </si>
+  <si>
+    <t>6 POS Header</t>
+  </si>
+  <si>
+    <t>HEADER 6P MINIFIT</t>
+  </si>
+  <si>
+    <t>39-30-1060</t>
+  </si>
+  <si>
+    <t>WM1353-ND</t>
+  </si>
+  <si>
+    <t>538-39-30-1060</t>
   </si>
 </sst>
 </file>
@@ -1992,8 +1992,8 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2009,6 +2009,7 @@
     <col min="16" max="16" width="27.375" customWidth="1"/>
     <col min="17" max="17" width="28" customWidth="1"/>
     <col min="18" max="18" width="22.375" customWidth="1"/>
+    <col min="19" max="19" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" thickBot="1">
@@ -4823,58 +4824,58 @@
         <v>1</v>
       </c>
       <c r="B54" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="I54" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="K54" s="6">
-        <v>0.33</v>
-      </c>
-      <c r="L54" s="6">
-        <v>0.38200000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="L54" s="22">
+        <v>0.88200000000000001</v>
       </c>
       <c r="M54" s="6">
         <f>K54*A54</f>
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N54" s="6">
         <f>L54*A54</f>
-        <v>0.38200000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="O54" s="4"/>
       <c r="P54" s="4" t="str">
-        <f>IF(NOT(I54=""),A54&amp;","&amp;I54,"")</f>
-        <v>1,WM3702-ND</v>
+        <f t="shared" ref="P54" si="19">IF(NOT(I54=""),A54&amp;","&amp;I54,"")</f>
+        <v>1,WM1353-ND</v>
       </c>
       <c r="Q54" t="str">
-        <f>A54&amp;"x "&amp;C54</f>
-        <v>1x 6-POS connector</v>
+        <f t="shared" ref="Q54" si="20">A54&amp;"x "&amp;C54</f>
+        <v>1x 6 POS Header</v>
       </c>
       <c r="R54" t="str">
-        <f>IF(NOT(J54=""),J54&amp;"|"&amp;A54,"")</f>
-        <v>538-39-01-2060|1</v>
+        <f t="shared" ref="R54" si="21">IF(NOT(J54=""),J54&amp;"|"&amp;A54,"")</f>
+        <v>538-39-30-1060|1</v>
       </c>
       <c r="S54" t="str">
-        <f>H54&amp;" "&amp;A54</f>
-        <v>39-01-2060 1</v>
+        <f t="shared" ref="S54" si="22">H54&amp;" "&amp;A54</f>
+        <v>39-30-1060 1</v>
       </c>
     </row>
     <row r="56" spans="1:19">

</xml_diff>

<commit_message>
Add diodes D6 D7 D8 & D13 to the BOM
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev2.2 documents/BOM-speeduino compatible PCB for m52 rev2.2.xlsx
+++ b/m52 PnP/Rev2.2 documents/BOM-speeduino compatible PCB for m52 rev2.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev2.2 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E096E9-A4AA-46BA-AA22-0E36447A9D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A2B9F5-5F3C-464D-8C15-E229132D609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29025" yWindow="4950" windowWidth="28650" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="1980" windowWidth="27975" windowHeight="15570" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -912,19 +912,6 @@
     <t>R9,R12,R15,R18,R46,R53</t>
   </si>
   <si>
-    <r>
-      <t>D3,D4,D9,D10,D11,D12,D18,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>D20</t>
-    </r>
-  </si>
-  <si>
     <t>Gate Drivers</t>
   </si>
   <si>
@@ -1253,6 +1240,19 @@
   </si>
   <si>
     <t>538-39-30-1060</t>
+  </si>
+  <si>
+    <r>
+      <t>D3,D4,D6,D7,D8,D9,D10,D11,D12,D13,D18,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>D20</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1993,7 +1993,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2223,7 +2223,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -2347,7 +2347,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -2409,7 +2409,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -2471,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
@@ -2686,7 +2686,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>88</v>
@@ -2867,10 +2867,10 @@
     <row r="16" spans="1:19" ht="26.25" thickBot="1">
       <c r="A16" s="16">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>240</v>
+        <v>302</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
@@ -2902,28 +2902,28 @@
       </c>
       <c r="M16" s="6">
         <f>K16*A16</f>
-        <v>0.88</v>
+        <v>1.32</v>
       </c>
       <c r="N16" s="6">
         <f>L16*A16</f>
-        <v>0.88</v>
+        <v>1.32</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>8,1N4004-TPMSCT-ND</v>
+        <v>12,1N4004-TPMSCT-ND</v>
       </c>
       <c r="Q16" t="str">
         <f>"Diode - " &amp;A16&amp;"x "&amp;C16</f>
-        <v>Diode - 8x 1N4004</v>
+        <v>Diode - 12x 1N4004</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="4"/>
-        <v>833-1N4004-TP|8</v>
+        <v>833-1N4004-TP|12</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="5"/>
-        <v>1N4004-TP 8</v>
+        <v>1N4004-TP 12</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" thickBot="1">
@@ -3114,10 +3114,10 @@
         <v>180</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -3125,13 +3125,13 @@
         <v>182</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K21" s="6">
         <v>1</v>
@@ -3259,7 +3259,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>85</v>
@@ -3583,7 +3583,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>43</v>
@@ -3705,7 +3705,7 @@
         <v>13</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C32" s="3">
         <v>470</v>
@@ -3765,7 +3765,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>154</v>
@@ -3827,7 +3827,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>87</v>
@@ -3955,21 +3955,21 @@
         <v>150</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="K36" s="5">
         <v>0.27</v>
@@ -4009,7 +4009,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>170</v>
@@ -4026,7 +4026,7 @@
         <v>172</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>173</v>
@@ -4224,7 +4224,7 @@
         <v>201</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
@@ -4286,7 +4286,7 @@
         <v>68</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
@@ -4404,10 +4404,10 @@
         <v>119</v>
       </c>
       <c r="C44" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>222</v>
@@ -4417,13 +4417,13 @@
         <v>148</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K44" s="6">
         <v>2.4</v>
@@ -4463,13 +4463,13 @@
         <v>2</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>202</v>
@@ -4479,13 +4479,13 @@
         <v>38</v>
       </c>
       <c r="H45" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="I45" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="J45" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="K45" s="6">
         <v>1.41</v>
@@ -4547,7 +4547,7 @@
     <row r="47" spans="1:19" ht="16.5" thickBot="1">
       <c r="A47" s="14"/>
       <c r="B47" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -4576,27 +4576,27 @@
         <v>13</v>
       </c>
       <c r="B48" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="H48" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="I48" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="I48" s="11" t="s">
+      <c r="J48" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="K48" s="6">
         <v>0.55000000000000004</v>
@@ -4638,10 +4638,10 @@
         <v>208</v>
       </c>
       <c r="C49" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="11"/>
@@ -4649,13 +4649,13 @@
         <v>182</v>
       </c>
       <c r="H49" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="K49" s="6">
         <v>0.33</v>
@@ -4700,7 +4700,7 @@
         <v>210</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="11"/>
@@ -4708,13 +4708,13 @@
         <v>182</v>
       </c>
       <c r="H50" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="K50" s="6">
         <v>0.16</v>
@@ -4769,7 +4769,7 @@
     <row r="52" spans="1:19" ht="16.5" thickBot="1">
       <c r="A52" s="14"/>
       <c r="B52" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -4785,10 +4785,10 @@
       <c r="N52" s="6"/>
       <c r="O52" s="9"/>
       <c r="P52" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R52" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
@@ -4796,18 +4796,18 @@
         <v>1</v>
       </c>
       <c r="B53" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D53" s="29" t="s">
         <v>294</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>295</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
@@ -4824,13 +4824,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -4838,13 +4838,13 @@
         <v>182</v>
       </c>
       <c r="H54" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="I54" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="I54" s="24" t="s">
+      <c r="J54" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="K54" s="6">
         <v>1</v>

</xml_diff>